<commit_message>
fixup! mira el comentario
</commit_message>
<xml_diff>
--- a/src/HDI.xlsx
+++ b/src/HDI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpereirar/Documents/Ongoing_publications/MulticriteriaClustering/Otros metodos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpereirar/Documents/GitHub/mcda/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AAEDFD-F5B3-3344-8F34-006863172866}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851ED6E6-6080-0D47-ADEC-178CED935BD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="27640" windowHeight="15440" xr2:uid="{31DC8480-D239-2045-A0F3-65C89ECF59A8}"/>
+    <workbookView xWindow="2860" yWindow="460" windowWidth="27640" windowHeight="15440" xr2:uid="{31DC8480-D239-2045-A0F3-65C89ECF59A8}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E192" sqref="E192:G192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2510,24 +2510,24 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="3">
-        <v>68.745999999999995</v>
+        <v>61.9</v>
       </c>
       <c r="B192" s="3">
-        <v>13.552050000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C192" s="3">
-        <v>7.8588618039999991</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="3">
-        <v>76.716499999999996</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="B193" s="3">
-        <v>17.827885000000002</v>
+        <v>16.5</v>
       </c>
       <c r="C193" s="3">
-        <v>10.995505901999998</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>